<commit_message>
Include SMS costs map in dynamic landscape facility
The facility to change the input SMS costs map is provided in batch mode only as part of the dynamic landscape feature; the costs may be changed simultaneously with other landscape changes or independently of them. For the GUI, there remains no option to change the cost map during the course of a simulation.
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/Batch_error_codes.xlsx
+++ b/doc/Manual/Batchmode/Batch_error_codes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter_v2_0\doc\Manual\Batchmode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32506691-2EA5-495D-B416-4A5A24C90FC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error codes" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Error in the landscape file: Invalid dimensions. ensure X &amp; Y are powers of 2 + 1.</t>
   </si>
@@ -159,12 +160,18 @@
   </si>
   <si>
     <t>Origin of cost map file differs from origin of landscape</t>
+  </si>
+  <si>
+    <t>Failed to open landscape costs file in readLandChange()</t>
+  </si>
+  <si>
+    <t>Invalid SMS cost read from costs file in readLandChange()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -486,8 +493,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -574,7 +581,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -582,7 +589,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -590,231 +597,231 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>300</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>301</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>400</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>440</v>
+        <v>403</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>500</v>
+        <v>434</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>501</v>
+        <v>440</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
+        <v>502</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>503</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>504</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>505</v>
-      </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>507</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -822,65 +829,81 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>601</v>
+        <v>509</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>602</v>
+        <v>510</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>901</v>
+        <v>602</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
+        <v>603</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>901</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>902</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update folder 'doc' as well to be in line with master
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/Batch_error_codes.xlsx
+++ b/doc/Manual/Batchmode/Batch_error_codes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter_v2_0\doc\Manual\Batchmode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32506691-2EA5-495D-B416-4A5A24C90FC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error codes" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Error in the landscape file: Invalid dimensions. ensure X &amp; Y are powers of 2 + 1.</t>
   </si>
@@ -159,12 +160,18 @@
   </si>
   <si>
     <t>Origin of cost map file differs from origin of landscape</t>
+  </si>
+  <si>
+    <t>Failed to open landscape costs file in readLandChange()</t>
+  </si>
+  <si>
+    <t>Invalid SMS cost read from costs file in readLandChange()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -486,8 +493,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -574,7 +581,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -582,7 +589,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -590,231 +597,231 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>300</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>301</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>400</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>440</v>
+        <v>403</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>500</v>
+        <v>434</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>501</v>
+        <v>440</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
+        <v>502</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>503</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>504</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>505</v>
-      </c>
-      <c r="B39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>507</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -822,65 +829,81 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>601</v>
+        <v>509</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>602</v>
+        <v>510</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>901</v>
+        <v>602</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
+        <v>603</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>901</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>902</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>